<commit_message>
Update 网站结构 v2 with danny edits.xlsx
</commit_message>
<xml_diff>
--- a/Design/xlsx/网站结构 v2 with danny edits.xlsx
+++ b/Design/xlsx/网站结构 v2 with danny edits.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donaldzou/Desktop/工作室/Site-Design/xlsx/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/donaldzou/Desktop/工作室/School-Platform/Design/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D02E2719-021C-5446-BB07-2F4BFA0E91FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{492E584B-622D-014D-B282-9A1DFC891BC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36100" yWindow="1240" windowWidth="33600" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37220" yWindow="1740" windowWidth="33600" windowHeight="19860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -776,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB180"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1072,89 +1072,98 @@
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="C32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C32" s="5"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1" t="s">
+      <c r="B33" s="5"/>
+      <c r="C33" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1" t="s">
+      <c r="B34" s="5"/>
+      <c r="C34" s="5" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1" t="s">
+      <c r="B35" s="5"/>
+      <c r="C35" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="1"/>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C36" s="1"/>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="5"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1" t="s">
+      <c r="B37" s="5"/>
+      <c r="C37" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1" t="s">
+      <c r="B38" s="5"/>
+      <c r="C38" s="5" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C39" s="1" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B39" s="4"/>
+      <c r="C39" s="5" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="4" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C41" s="1" t="s">
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B41" s="4"/>
+      <c r="C41" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C42" s="1" t="s">
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B42" s="4"/>
+      <c r="C42" s="5" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C43" s="1" t="s">
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B43" s="4"/>
+      <c r="C43" s="5" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B44" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C45" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C46" s="1" t="s">
         <v>62</v>
       </c>

</xml_diff>